<commit_message>
rough of several revisions
</commit_message>
<xml_diff>
--- a/document/revisions.xlsx
+++ b/document/revisions.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>feedback</t>
   </si>
@@ -134,9 +135,6 @@
     <t>clarify that problem space manipulation transforms solution representation, not the problem instance</t>
   </si>
   <si>
-    <t>discussion on whether or not to replan at all, and, if so, how to select appropriate algorithm</t>
-  </si>
-  <si>
     <t>future work - discussion on distributed planning</t>
   </si>
   <si>
@@ -165,6 +163,39 @@
   </si>
   <si>
     <t>done. Added clarifications and explicit statement in sec 4.3.2</t>
+  </si>
+  <si>
+    <t>continuous domain would require use of number of samples rather than sample rate</t>
+  </si>
+  <si>
+    <t>done.  utility loss explained in ch 4 intro. Added description of sample rate in ch 4 intro</t>
+  </si>
+  <si>
+    <t>multiple agents attempting to solve a task can be represented as a distributed planning problem.  Particularly when there is limited communication, the actions of one agent can be represented as environmental uncertainty.  PSA techniques could be used to help an agent anticipate and/or plan for the potential actions of other agents.    Not specific to distributed planning, but an agent could use PSA to preference it towards situations in which there are less possible plans, resulting in less volitile replanning.  This would lessen the impact of a partnering agent that behaves unexpectedly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSS is most readily parallelized.  The planning space can be divided between the available processors and a copy of the known solution can be provided to each.  Each processor can then test its section of the planning space against each solution and emit the best solution for each planning instance.    The initial sampling step which is common to each of the algorithms could be parallelized by dividing the planning space between k processors and allocating total samples/k to each processor.  The centralized version of the algorithm will be a normally distributed sample, and dividing the space in the manner will not affect htat.  However, the possibility of obtaining some skewed sample by chance would be diminished.  </t>
+  </si>
+  <si>
+    <t>discussion on whether or not to replan at all, and, if so, whether to use online repair vs PSA</t>
+  </si>
+  <si>
+    <t>if plan remains feasible, and the utility loss is tolerable, then there is no need to replan.  If not, then the choice between PSA and online repair can be determined by the equations in ch 5</t>
+  </si>
+  <si>
+    <t>clustering is a function of low number of solutions in the space, leading to low numbers of permutations of discovered solutions during the initial sampling stage.  The performance of the algorithms is sensitive to the solutions discovered.  Thus the same permutation tends to lead to similar performance of the algorithm, resulting in clustering.</t>
+  </si>
+  <si>
+    <t>same as 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">example of losing some percentage of computing resources.  One could imagine that if a missile hits a ship, then the scope of possible reallocation problems is not very granular.  Thus one would not have to plan for each of the permutation of servers A though Z becoming unavailable.  Rather, the planner would consider broader effects of damage to clusters of servers such as A-M going down and N-Z going down.  Therefore the permuations are fewer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In the mine line object scenario, reports of MLOs come in slowly enough where one can consider the problem similar to the TSP experiments, where only one new location has to be considered.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS Maps give a view of how frequently alternate plans occur within a range of variable attributes within the scope of possible environment changes.  Particularly in cases in which the alternate plan is very different from the current plan, this could be valuable for allowing a system to prepare for switching to that plan.   A PS Map could also assist in identifying environemt changes that are more lilely to trigger the need for an alternative plan, thus if there are resources available to mitigate that change, then this information would allow them to be deployed most appropriately.  For example, if a PS Map were to demonstrate that modifying a TSP route to accomodate new location A is more disruptive than accomodating new location B, then steps could be taken the prevent the need for location A, or to acquire additional information about the possibility of location A, and perhaps determine that preparing for that possibility is not necessary.   </t>
   </si>
 </sst>
 </file>
@@ -516,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,9 +558,12 @@
     <col min="1" max="1" width="27.5546875" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.109375" style="1" customWidth="1"/>
+    <col min="6" max="13" width="18.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -539,8 +573,18 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -551,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -562,7 +606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>A3+1</f>
         <v>4</v>
@@ -571,7 +615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" ref="A5:A6" si="0">A4+1</f>
         <v>5</v>
@@ -583,7 +627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -595,19 +639,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -615,7 +672,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>A9+1</f>
         <v>10</v>
@@ -624,10 +681,10 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" ref="A11:A20" si="1">A10+1</f>
         <v>11</v>
@@ -636,10 +693,10 @@
         <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -648,37 +705,46 @@
         <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -686,48 +752,73 @@
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -738,7 +829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -749,7 +840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24">
         <f>A23+1</f>
         <v>24</v>
@@ -761,7 +852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" ref="A25:A38" si="2">A24+1</f>
         <v>25</v>
@@ -773,7 +864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -785,7 +876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -797,7 +888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -806,7 +897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -815,7 +906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -824,7 +915,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -836,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -845,7 +936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -854,7 +945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -862,8 +953,11 @@
       <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -872,7 +966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -881,7 +975,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -890,7 +984,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="2"/>
         <v>38</v>

</xml_diff>

<commit_message>
addl work on revision 8 - continuous domain
</commit_message>
<xml_diff>
--- a/document/revisions.xlsx
+++ b/document/revisions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>feedback</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>discussed in 16</t>
+  </si>
+  <si>
+    <t>done. added note in ch4 TSP domain description.  Added discussion on continuous domains in future work</t>
+  </si>
+  <si>
+    <t>done.  Added section to future work</t>
+  </si>
+  <si>
+    <t>TSP and knapsack are made discrete for this work.  Elevator is a discrete domain.  Adversarial problems:  Non contiguous solution spaces could fool SBE-trace</t>
+  </si>
+  <si>
+    <t>done. Added description in sec 5.2</t>
   </si>
 </sst>
 </file>
@@ -555,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,6 +678,9 @@
       <c r="B8" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>46</v>
       </c>
@@ -758,6 +773,9 @@
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>52</v>
       </c>
@@ -769,6 +787,9 @@
       </c>
       <c r="B17" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>49</v>
@@ -974,6 +995,9 @@
       <c r="B35" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A36">
@@ -1003,6 +1027,9 @@
       </c>
       <c r="B38" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
distributed planning, addl description of fig 4.1, addl sbe description, example motivational domain, explanation of timing graph clustering, discussion on if to replan at all
</commit_message>
<xml_diff>
--- a/document/revisions.xlsx
+++ b/document/revisions.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>feedback</t>
   </si>
@@ -117,9 +116,6 @@
     <t>I'd like to see some discussion on scale-- i.e., making the problem domains harder or bigger. It doesn't need to be backed up by experiments, I just want to have the idea of how this might scale to be intuitively explained. How does time complexity and memory complexity relate to sample size (or compute time) and average utility loss? Is it polynomial or exponential? Can larger problems be overcome by parallelism?</t>
   </si>
   <si>
-    <t>here were a bunch of graphs and visualizations that were in the presentation that should find their way into the dissertation. Many of them were very useful in understanding it better.</t>
-  </si>
-  <si>
     <t>I'd be interested in seeing a more clear outline of assumptions early on in the text, such as the domains are discrete. Also, perhaps discuss which domains or "adversarial" problems could really cause your algorithm some heartache (think of the spiral galaxy case).</t>
   </si>
   <si>
@@ -165,9 +161,6 @@
     <t>done. Added clarifications and explicit statement in sec 4.3.2</t>
   </si>
   <si>
-    <t>continuous domain would require use of number of samples rather than sample rate</t>
-  </si>
-  <si>
     <t>done.  utility loss explained in ch 4 intro. Added description of sample rate in ch 4 intro</t>
   </si>
   <si>
@@ -180,18 +173,12 @@
     <t>discussion on whether or not to replan at all, and, if so, whether to use online repair vs PSA</t>
   </si>
   <si>
-    <t>if plan remains feasible, and the utility loss is tolerable, then there is no need to replan.  If not, then the choice between PSA and online repair can be determined by the equations in ch 5</t>
-  </si>
-  <si>
     <t>clustering is a function of low number of solutions in the space, leading to low numbers of permutations of discovered solutions during the initial sampling stage.  The performance of the algorithms is sensitive to the solutions discovered.  Thus the same permutation tends to lead to similar performance of the algorithm, resulting in clustering.</t>
   </si>
   <si>
     <t xml:space="preserve">example of losing some percentage of computing resources.  One could imagine that if a missile hits a ship, then the scope of possible reallocation problems is not very granular.  Thus one would not have to plan for each of the permutation of servers A though Z becoming unavailable.  Rather, the planner would consider broader effects of damage to clusters of servers such as A-M going down and N-Z going down.  Therefore the permuations are fewer. </t>
   </si>
   <si>
-    <t xml:space="preserve"> In the mine line object scenario, reports of MLOs come in slowly enough where one can consider the problem similar to the TSP experiments, where only one new location has to be considered.</t>
-  </si>
-  <si>
     <t xml:space="preserve">PS Maps give a view of how frequently alternate plans occur within a range of variable attributes within the scope of possible environment changes.  Particularly in cases in which the alternate plan is very different from the current plan, this could be valuable for allowing a system to prepare for switching to that plan.   A PS Map could also assist in identifying environemt changes that are more lilely to trigger the need for an alternative plan, thus if there are resources available to mitigate that change, then this information would allow them to be deployed most appropriately.  For example, if a PS Map were to demonstrate that modifying a TSP route to accomodate new location A is more disruptive than accomodating new location B, then steps could be taken the prevent the need for location A, or to acquire additional information about the possibility of location A, and perhaps determine that preparing for that possibility is not necessary.   </t>
   </si>
   <si>
@@ -214,13 +201,49 @@
   </si>
   <si>
     <t>done. Added description in sec 5.2</t>
+  </si>
+  <si>
+    <t>continuous domain would require use of number of samples rather than sample rate.  All algs could work in an approximated continous domain.  A truly continuous domain could be supported by modifications to SSS, SBE, SVM, and SVM+SBE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In the mine like object scenario, reports of MLOs come in slowly enough where one can consider the problem similar to the TSP experiments, where only one new location has to be considered.</t>
+  </si>
+  <si>
+    <t>there were a bunch of graphs and visualizations that were in the presentation that should find their way into the dissertation. Many of them were very useful in understanding it better.</t>
+  </si>
+  <si>
+    <t>intuitively, I would guess logarithmically.  Improvement seems to steady until the sample rate reaches a critical mass at which point additional improvement becomes unlikely.  However, I would imagine a high degree of variability due to the stochastic nature of the problem.  If a sample happens upon a key solution, or provides some key information regarding a solution border, then that specific sample could greatly improve the performance of that instance of the algorithm.  Thus the improvement could vary widely with each sample, and of course with each domain and the specific problem instance.</t>
+  </si>
+  <si>
+    <t>if the current plan remains feasible, and the utility loss is tolerable, then there is no need to replan.  If not, then the choice between PSA and online repair can be determined by the equations in ch 5.  Future work could consider factoring in externalities such as  cost of swtiching plans, allowing for situations in which a suboptimal plan is preferable to a high cost of switching.</t>
+  </si>
+  <si>
+    <t>done.  Added text to tradeoff with online repair in Ch 5</t>
+  </si>
+  <si>
+    <t>done.  Added distributed planning section in future work</t>
+  </si>
+  <si>
+    <t>done.  Added to introduction</t>
+  </si>
+  <si>
+    <t>done.  Added more explicit description to caption and confirmed descriptive text in references to figure</t>
+  </si>
+  <si>
+    <t>initial drafted notes</t>
+  </si>
+  <si>
+    <t>done. Added initial paragraph at beginning of SBE description</t>
+  </si>
+  <si>
+    <t>This next technique differs from previous algorithms in that instead of using a nearest neighbor approach to classify unsolved problem instances to known solutions, this technique uses the problem domain's objective function to find the borders between solutions, thus allowing it to classify all the problem instances within a region.  The intent is that this technique will be more accurate than the previous algorithms, but does require the availability of an objective function and can be more computationally expensive.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +266,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +293,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -267,11 +308,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -284,9 +326,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,7 +644,9 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -676,22 +731,33 @@
         <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
+    </row>
+    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -699,10 +765,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -711,10 +777,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -723,22 +789,25 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -747,10 +816,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -759,10 +831,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -774,10 +846,10 @@
         <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -786,13 +858,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -800,27 +872,40 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
+      <c r="B18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="7" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="B19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -828,10 +913,13 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -918,25 +1006,42 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="28" spans="1:13" s="9" customFormat="1" ht="121.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="C28" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="7" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -944,6 +1049,9 @@
       <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C30" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -957,7 +1065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -965,17 +1073,31 @@
       <c r="B32" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="D32" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -983,11 +1105,14 @@
       <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C34" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D34" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -996,41 +1121,72 @@
         <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A36">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="C36" s="8"/>
+      <c r="D36" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="1:13" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="1:13" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
all revisions except baseline in graphs
</commit_message>
<xml_diff>
--- a/document/revisions.xlsx
+++ b/document/revisions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>feedback</t>
   </si>
@@ -50,9 +50,6 @@
     <t>add online repair baseline to figures</t>
   </si>
   <si>
-    <t>clarify explanation of SVM alg in sec 4.1.9</t>
-  </si>
-  <si>
     <t>justification of SVM+SBE alpha values in sec 4.1.9</t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>does loss from optimal improve logarithmically, exponentially, or quadratrically as sample rate increases?</t>
   </si>
   <si>
-    <t>error bars or variance metric to help compare alg performance</t>
-  </si>
-  <si>
     <t>description of clustering in timing graphs</t>
   </si>
   <si>
@@ -182,12 +176,6 @@
     <t xml:space="preserve">PS Maps give a view of how frequently alternate plans occur within a range of variable attributes within the scope of possible environment changes.  Particularly in cases in which the alternate plan is very different from the current plan, this could be valuable for allowing a system to prepare for switching to that plan.   A PS Map could also assist in identifying environemt changes that are more lilely to trigger the need for an alternative plan, thus if there are resources available to mitigate that change, then this information would allow them to be deployed most appropriately.  For example, if a PS Map were to demonstrate that modifying a TSP route to accomodate new location A is more disruptive than accomodating new location B, then steps could be taken the prevent the need for location A, or to acquire additional information about the possibility of location A, and perhaps determine that preparing for that possibility is not necessary.   </t>
   </si>
   <si>
-    <t>for knapsack, likely not an issue w/r/t alg performance since items that are not "better" than an item already in the sack are not included in the knapsack.  Thus there tend to be less disruption of the current plan compared to a domain like TSP.  In TSP, additional locations increase dimensionality linearly as well.  However, the because the new locations must be included in the plan, more plans will be in the space.  It is not clear if that space would amenible to the algorithms.  Space and time considerations?  PS Map would potentially require more space, although more efficient representations are possible.  Quad trees, for example.  Also, one doesn't necessarily have to store the complete map.  A SVM solution could just store the model, and an SSS solution can just store a list of all the solutions in the space.  Time?  Polynomial increase as depicted in Table 3.1</t>
-  </si>
-  <si>
-    <t>parallelism discussed in 17, scale discussed in 19</t>
-  </si>
-  <si>
     <t>discussed in 16</t>
   </si>
   <si>
@@ -197,9 +185,6 @@
     <t>done.  Added section to future work</t>
   </si>
   <si>
-    <t>TSP and knapsack are made discrete for this work.  Elevator is a discrete domain.  Adversarial problems:  Non contiguous solution spaces could fool SBE-trace</t>
-  </si>
-  <si>
     <t>done. Added description in sec 5.2</t>
   </si>
   <si>
@@ -237,6 +222,102 @@
   </si>
   <si>
     <t>This next technique differs from previous algorithms in that instead of using a nearest neighbor approach to classify unsolved problem instances to known solutions, this technique uses the problem domain's objective function to find the borders between solutions, thus allowing it to classify all the problem instances within a region.  The intent is that this technique will be more accurate than the previous algorithms, but does require the availability of an objective function and can be more computationally expensive.</t>
+  </si>
+  <si>
+    <t>parallelism discussed in 17, scale discussed in 19.  Re improvement in performance as function of sample size, my intuition is that it would resemble a sigmoid function.  As the number of samples increase the performance slowly increases until the number of samples reaches a critical mass at which point performance increases rapidly until performance levels off.</t>
+  </si>
+  <si>
+    <t>done.  Added a brief summary of the algorithm before  its complexity analysis</t>
+  </si>
+  <si>
+    <t>done.  Added in chapter 3</t>
+  </si>
+  <si>
+    <t>done.  Added to chapter 3</t>
+  </si>
+  <si>
+    <t>TSP and knapsack are made discrete for this work.  Elevator is a discrete domain.  Adversarial problems:   Small or non existant solution regions would cause problem for all algorithms except perhaps a purely mathematical implementation of SBE.  Neighboring solution regions with large difference in utility would negatively impact performance.</t>
+  </si>
+  <si>
+    <t>added comment about discrete version of domain to TSP and knapsack domain descriptions.  Added thoughts about challenging domains to chapter 5 algorithmic assumptions section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  As the problem space grows, algorithms that solve large portions of the unsolved problem instances at once, rather than individual problem instances, become more important.  The solution border estimation (SBE) and the support vector machine (SVM) algorithms attempt to find solutions to large regions of the space, and thus could be viable when considering more complex problem domains.  Space and time considerations?  PS Map would potentially require more space, although more efficient representations are possible.  Quad trees, for example.  Also, one doesn't necessarily have to store the complete map.  A SVM solution could just store the model, and an SSS solution can just store a list of all the solutions in the space.  Time?  Polynomial increase as depicted in Table 3.1</t>
+  </si>
+  <si>
+    <t>add section in chapter 5</t>
+  </si>
+  <si>
+    <t>added section in chapter 5 regarding scalability</t>
+  </si>
+  <si>
+    <t>added a paragraph in chapter 5 in the scalability section</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>clarify explanation of SVM alg in sec 4.1.7</t>
+  </si>
+  <si>
+    <t>53-54</t>
+  </si>
+  <si>
+    <t>47,103-104</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>17-19,59-62</t>
+  </si>
+  <si>
+    <t>89-90</t>
+  </si>
+  <si>
+    <t>107-108</t>
+  </si>
+  <si>
+    <t>46-47</t>
+  </si>
+  <si>
+    <t>94-95</t>
+  </si>
+  <si>
+    <t>106-107</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>98-101</t>
+  </si>
+  <si>
+    <t>108-109</t>
+  </si>
+  <si>
+    <t>14-15</t>
+  </si>
+  <si>
+    <t>20-21</t>
+  </si>
+  <si>
+    <t>33-34</t>
+  </si>
+  <si>
+    <t>40-44</t>
+  </si>
+  <si>
+    <t>50, various</t>
+  </si>
+  <si>
+    <t>86-87</t>
+  </si>
+  <si>
+    <t>103-104</t>
+  </si>
+  <si>
+    <t>pages (logical)</t>
   </si>
 </sst>
 </file>
@@ -313,7 +394,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -326,15 +407,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -618,36 +741,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="2" max="2" width="46" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="73" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.109375" style="1" customWidth="1"/>
-    <col min="6" max="13" width="18.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="46" style="15" customWidth="1"/>
+    <col min="3" max="3" width="34.77734375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="13" style="19" customWidth="1"/>
+    <col min="5" max="5" width="73" style="15" customWidth="1"/>
+    <col min="6" max="6" width="42.109375" style="1" customWidth="1"/>
+    <col min="7" max="14" width="18.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="D1" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -656,67 +782,93 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="D2" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="D3" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="6" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
         <f>A3+1</f>
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="C4" s="17"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
         <f t="shared" ref="A5:A6" si="0">A4+1</f>
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="D5" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="D6" s="19">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -725,208 +877,232 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="15" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <f>A9+1</f>
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="B10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <f t="shared" ref="A11:A20" si="1">A10+1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="B11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="B12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="19">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="B13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="144.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="B14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="B15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="B16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="175.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="B17" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="7" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+      <c r="B18" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="15" customFormat="1" ht="193.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-    </row>
-    <row r="20" spans="1:13" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="B19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="B20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -935,258 +1111,260 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>23</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="D23" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
         <f>A23+1</f>
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <f t="shared" ref="A25:A37" si="2">A24+1</f>
+        <v>25</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <f t="shared" ref="A25:A38" si="2">A24+1</f>
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="C25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="B26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="9" customFormat="1" ht="121.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="B27" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="8" customFormat="1" ht="121.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="7" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
+      <c r="B28" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="15" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-    </row>
-    <row r="30" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="B29" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="B30" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="D31" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="15" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
+      <c r="B32" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="19">
+        <v>101</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="B33" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="B34" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="15" customFormat="1" ht="153.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="15">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" s="7" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
+      <c r="B35" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="15" customFormat="1" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-    </row>
-    <row r="37" spans="1:13" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7">
+      <c r="B36" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="15" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-    </row>
-    <row r="38" spans="1:13" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
+      <c r="B37" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>